<commit_message>
Updated with Gabel's script, Kasi still having some issues
</commit_message>
<xml_diff>
--- a/urc_tables/2022.xlsx
+++ b/urc_tables/2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My_Projects\HEPB_Rotation\FRM_Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Watersheds\HEPB_2022_AERTSR_Updates-Gabel\frm_tool_urc_to_dss\urc_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88B9AB4-7473-40B2-AA31-DF6BBDE508DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AEFBA5-5424-45EF-9EEB-4F1D3A4641F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7EB13AD6-5E71-4CEF-98B5-115A795515F5}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" activeTab="4" xr2:uid="{7EB13AD6-5E71-4CEF-98B5-115A795515F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,17 @@
     <sheet name="Apr" sheetId="2" r:id="rId5"/>
     <sheet name="May" sheetId="3" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="eaalf">#REF!</definedName>
+    <definedName name="eaard">#REF!</definedName>
+    <definedName name="eabrn">#REF!</definedName>
+    <definedName name="eadcd">#REF!</definedName>
+    <definedName name="eadwr">#REF!</definedName>
+    <definedName name="eagcl">#REF!</definedName>
+    <definedName name="eahgh">#REF!</definedName>
+    <definedName name="eaker">#REF!</definedName>
+    <definedName name="ealib">#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t xml:space="preserve">         units   Oct 31  Nov 30  Dec 31  Jan 31  Feb 28  Mar 31  Apr 15  Apr 30  May 31  Jun 30  Jul 31  Aug 31  Sep 30</t>
   </si>
@@ -74,25 +85,76 @@
     <t>ALF         ft   2062.5  2062.5  2062.5  2060.0  2060.0  2056.0     n/a  2056.0  2062.5  2062.5  2062.5  2062.5  2062.5</t>
   </si>
   <si>
-    <t>MCDB       kaf      200     200     390    1662    2810    4080    4080    4080    2448       0       0       0       0</t>
-  </si>
-  <si>
-    <t>ARDB        ft   1442.0  1442.0  1438.5  1430.5  1422.9  1414.1  1414.1  1414.1  1423.9  1443.2  1444.0  1444.0  1444.0</t>
-  </si>
-  <si>
-    <t>LIB         ft   2459.0  2448.0  2411.0  2388.9  2370.5  2363.2  2363.2  2363.2  2422.1  2459.0  2459.0  2459.0  2459.0</t>
-  </si>
-  <si>
     <t>HGH         ft   3555.8  3555.8  3549.0  3544.1  3539.4  3534.1  3531.4  3528.8  3552.6  3560.0  3560.0  3560.0  3560.0</t>
   </si>
   <si>
-    <t>GCL         ft   1290.0  1290.0  1290.0  1290.0  1290.0  1281.8  1269.9  1257.9  1274.6  1289.7  1290.0  1290.0  1290.0</t>
-  </si>
-  <si>
-    <t>BRN         ft   2077.0  2077.0  2077.0  2077.0  2056.1  2057.8  2061.9  2062.8  2074.9  2077.0  2077.0  2077.0  2077.0</t>
-  </si>
-  <si>
-    <t>DWR         ft   1581.5  1568.8  1558.0  1527.6  1500.1  1459.9  1450.0  1490.4  1564.3  1599.0  1600.0  1600.0  1587.5</t>
+    <t>MCDB       kaf      200     200     390    1588    2685    3899    3899    3899    2340       0       0       0       0</t>
+  </si>
+  <si>
+    <t>ARDB        ft   1442.0  1442.0  1438.5  1429.9  1422.1  1412.9  1412.9  1412.9  1423.1  1443.1  1444.0  1444.0  1444.0</t>
+  </si>
+  <si>
+    <t>LIB         ft   2459.0  2448.0  2411.0  2407.0  2399.2  2391.4  2391.2  2391.0  2431.0  2459.0  2459.0  2459.0  2459.0</t>
+  </si>
+  <si>
+    <t>GCL         ft   1290.0  1290.0  1290.0  1290.0  1287.5  1263.0  1251.0  1239.0  1266.2  1289.6  1290.0  1290.0  1290.0</t>
+  </si>
+  <si>
+    <t>BRN         ft   2077.0  2077.0  2077.0  2077.0  2049.6  2045.4  2044.0  2042.6  2072.3  2077.0  2077.0  2077.0  2077.0</t>
+  </si>
+  <si>
+    <t>DWR         ft   1581.5  1568.8  1558.0  1536.7  1524.0  1512.5  1498.8  1523.8  1581.9  1600.0  1600.0  1600.0  1587.5</t>
+  </si>
+  <si>
+    <t>ARDB        ft   1442.0  1442.0  1438.5  1430.1  1422.9  1414.1  1414.1  1414.1  1423.9  1443.2  1444.0  1444.0  1444.0</t>
+  </si>
+  <si>
+    <t>LIB         ft   2459.0  2448.0  2411.0  2384.6  2363.9  2355.6  2355.6  2355.6  2419.9  2459.0  2459.0  2459.0  2459.0</t>
+  </si>
+  <si>
+    <t>HGH         ft   3555.8  3555.8  3549.0  3542.2  3539.3  3533.9  3531.2  3528.5  3552.5  3560.0  3560.0  3560.0  3560.0</t>
+  </si>
+  <si>
+    <t>GCL         ft   1290.0  1290.0  1290.0  1290.0  1290.0  1265.3  1248.7  1244.5  1268.6  1289.6  1290.0  1290.0  1290.0</t>
+  </si>
+  <si>
+    <t>BRN         ft   2077.0  2077.0  2077.0  2077.0  2053.7  2053.7  2056.4  2056.4  2074.0  2077.0  2077.0  2077.0  2077.0</t>
+  </si>
+  <si>
+    <t>DWR         ft   1581.5  1568.8  1558.0  1527.8  1518.6  1519.5  1527.2  1509.8  1571.0  1600.0  1600.0  1600.0  1587.5</t>
+  </si>
+  <si>
+    <t>MCDB       kaf      200     200     390    1609    2810    4080    4080    4080    2448       0       0       0       0</t>
+  </si>
+  <si>
+    <t>LIB         ft   2459.0  2448.0  2411.0  2384.6  2363.9  2371.8  2371.8  2371.8  2424.8  2459.0  2459.0  2459.0  2459.0</t>
+  </si>
+  <si>
+    <t>HGH         ft   3555.8  3555.8  3549.0  3542.2  3539.3  3539.3  3537.7  3536.0  3554.2  3560.0  3560.0  3560.0  3560.0</t>
+  </si>
+  <si>
+    <t>GCL         ft   1290.0  1290.0  1290.0  1290.0  1290.0  1271.5  1255.4  1249.9  1271.0  1289.6  1290.0  1290.0  1290.0</t>
+  </si>
+  <si>
+    <t>BRN         ft   2077.0  2077.0  2077.0  2077.0  2053.7  2059.1  2062.8  2064.1  2075.1  2077.0  2077.0  2077.0  2077.0</t>
+  </si>
+  <si>
+    <t>DWR         ft   1581.5  1568.8  1558.0  1527.8  1518.6  1528.6  1537.2  1517.8  1573.9  1600.0  1600.0  1600.0  1587.5</t>
+  </si>
+  <si>
+    <t>LIB         ft   2459.0  2448.0  2411.0  2384.6  2363.9  2371.8  2370.7  2370.7  2424.4  2459.0  2459.0  2459.0  2459.0</t>
+  </si>
+  <si>
+    <t>HGH         ft   3555.8  3555.8  3549.0  3542.2  3539.3  3539.3  3543.4  3542.5  3555.8  3560.0  3560.0  3560.0  3560.0</t>
+  </si>
+  <si>
+    <t>GCL         ft   1290.0  1290.0  1290.0  1290.0  1290.0  1271.5  1258.2  1250.7  1271.4  1289.6  1290.0  1290.0  1290.0</t>
+  </si>
+  <si>
+    <t>BRN         ft   2077.0  2077.0  2077.0  2077.0  2053.7  2059.1  2069.1  2077.0  2077.0  2077.0  2077.0  2077.0  2077.0</t>
+  </si>
+  <si>
+    <t>DWR         ft   1581.5  1568.8  1558.0  1527.8  1518.6  1528.6  1559.5  1540.0  1580.2  1600.0  1600.0  1600.0  1587.5</t>
   </si>
 </sst>
 </file>
@@ -454,7 +516,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,17 +528,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -486,7 +548,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -516,6 +578,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -523,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D175C2-5E9C-40E7-86FE-6C1C67AD7789}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,27 +649,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A2D5EC-509D-4D84-8023-B0B68E75AD84}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD79C18-5EFE-49E0-AF00-A92BCFD31AC4}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K16:K17"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,17 +670,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -638,22 +690,22 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -668,18 +720,147 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3291D549-60EE-4346-92BC-989A861A97D0}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD79C18-5EFE-49E0-AF00-A92BCFD31AC4}">
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3291D549-60EE-4346-92BC-989A861A97D0}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -692,5 +873,6 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>